<commit_message>
Userdata gets uploaded in DB, Events get created, Tokens are generated
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\WienerLinienEvent\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\Wiener-Linien-Event\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEE91933-FDDF-49EE-B577-82BFF636DB88}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12188405-2BCE-4E34-AC16-BC98D2404529}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11955" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,13 +34,13 @@
     <t>a.gruebling@gmail.com</t>
   </si>
   <si>
-    <t>6136@htl.rennweg.at</t>
-  </si>
-  <si>
     <t>Rafael</t>
   </si>
   <si>
     <t>Fiedler</t>
+  </si>
+  <si>
+    <t>6138@htl.rennweg.at</t>
   </si>
 </sst>
 </file>
@@ -392,7 +392,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -402,13 +402,13 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
         <v>5</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.45">

</xml_diff>